<commit_message>
Created PDF for blog
</commit_message>
<xml_diff>
--- a/computer-science/elixir-for-beginners/project_1/operators.xlsx
+++ b/computer-science/elixir-for-beginners/project_1/operators.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06af25a4dc2b6874/Documents/Blog/computer-science/elixir-for-beginners/project_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_F25DC773A252ABDACC104892795F5F2A5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{461B606A-98CE-433A-AD24-5BBAFA59D407}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_F25DC773A252ABDACC104892795F5F2A5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9D9A78A-7148-4806-B34E-E73441941D45}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="arithmetic" sheetId="1" r:id="rId1"/>
     <sheet name="comparison" sheetId="2" r:id="rId2"/>
+    <sheet name="logical" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Operator</t>
   </si>
@@ -122,6 +123,24 @@
   </si>
   <si>
     <t>Value is less than or equal to</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>Condition A and B are true</t>
+  </si>
+  <si>
+    <t>Condition A or B are true</t>
+  </si>
+  <si>
+    <t>Invert the boolean value</t>
   </si>
 </sst>
 </file>
@@ -175,6 +194,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -524,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEF64B2-E68B-4462-96E3-E44A73229CFB}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -656,4 +679,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045CADE3-418C-4F1A-9693-EB8AE45CDDD7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>